<commit_message>
adjust apical and basal distances
</commit_message>
<xml_diff>
--- a/references/minigland.xlsx
+++ b/references/minigland.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrug001/Desktop/nesi00119/mesh_2021/references/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477CF770-0E76-8943-B4C0-590E4404EE4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176A5996-3BB4-1941-ADC5-3D8CF2C084C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="1180" windowWidth="22520" windowHeight="23220" xr2:uid="{C018111C-319E-5144-81D0-8C90BCD3CB14}"/>
   </bookViews>
@@ -35,9 +35,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
-    <t>sd</t>
-  </si>
-  <si>
     <t>acinus</t>
   </si>
   <si>
@@ -83,9 +80,6 @@
     <t>cells in radial ring</t>
   </si>
   <si>
-    <t>Mini-gland structure measurement</t>
-  </si>
-  <si>
     <t>duct - outer</t>
   </si>
   <si>
@@ -93,6 +87,12 @@
   </si>
   <si>
     <t>apical to basal,  cuboid</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>Parotid gland measurement</t>
   </si>
 </sst>
 </file>
@@ -463,49 +463,49 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" customWidth="1"/>
-    <col min="3" max="3" width="5" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" customWidth="1"/>
     <col min="5" max="5" width="4.1640625" customWidth="1"/>
-    <col min="6" max="6" width="40" customWidth="1"/>
+    <col min="6" max="6" width="32.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5">
         <v>32.5</v>
@@ -514,12 +514,12 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>16.899999999999999</v>
@@ -534,12 +534,12 @@
         <v>1.5</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>0.77</v>
@@ -548,17 +548,17 @@
         <v>0.15</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>23.2</v>
@@ -567,12 +567,12 @@
         <v>3.3</v>
       </c>
       <c r="F10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11">
         <v>1.6</v>
@@ -581,12 +581,12 @@
         <v>0.25</v>
       </c>
       <c r="F11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12">
         <v>9.8000000000000007</v>
@@ -595,12 +595,12 @@
         <v>1.5</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13">
         <v>5</v>
@@ -611,12 +611,12 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>47.6</v>
@@ -625,12 +625,12 @@
         <v>5.2</v>
       </c>
       <c r="F16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17">
         <v>8</v>
@@ -639,12 +639,12 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="F17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B18">
         <v>18</v>
@@ -653,12 +653,12 @@
         <v>3.1</v>
       </c>
       <c r="F18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D19">
         <v>13</v>
@@ -669,7 +669,7 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21">
         <v>4.2</v>
@@ -678,7 +678,7 @@
         <v>0.59</v>
       </c>
       <c r="F21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>